<commit_message>
data updated on 2025-10-26 23:49:06.601496
</commit_message>
<xml_diff>
--- a/output/2025/scraped_data/Superintendency of Health 2025.xlsx
+++ b/output/2025/scraped_data/Superintendency of Health 2025.xlsx
@@ -1652,7 +1652,7 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Gestor de intereses</t>
+          <t>Lobista</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
@@ -2798,7 +2798,7 @@
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>asociacion de isapres de chile</t>
+          <t>ESENCIAL S.A.</t>
         </is>
       </c>
       <c r="N53" t="inlineStr">
@@ -3739,7 +3739,7 @@
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>Gestor de intereses</t>
+          <t>Lobista</t>
         </is>
       </c>
       <c r="M74" t="inlineStr">
@@ -3844,7 +3844,7 @@
       </c>
       <c r="M76" t="inlineStr">
         <is>
-          <t>asociacion de isapres de chile</t>
+          <t>ESENCIAL S.A.</t>
         </is>
       </c>
       <c r="N76" t="inlineStr">
@@ -4226,7 +4226,7 @@
       </c>
       <c r="L85" t="inlineStr">
         <is>
-          <t>Gestor de intereses</t>
+          <t>Lobista</t>
         </is>
       </c>
       <c r="M85" t="inlineStr">
@@ -5324,7 +5324,7 @@
       </c>
       <c r="M111" t="inlineStr">
         <is>
-          <t>asociacion de isapres de chile</t>
+          <t>ESENCIAL S.A.</t>
         </is>
       </c>
       <c r="N111" t="inlineStr">
@@ -6779,7 +6779,7 @@
       </c>
       <c r="M140" t="inlineStr">
         <is>
-          <t>Indra Sistemas Chile SA</t>
+          <t>Indra Sistemas Chile S.A.</t>
         </is>
       </c>
       <c r="N140" t="inlineStr">
@@ -7032,7 +7032,7 @@
       </c>
       <c r="M146" t="inlineStr">
         <is>
-          <t>Soluciones en Seguridad Limitada</t>
+          <t>Soluciones en Seguridad Ltda</t>
         </is>
       </c>
       <c r="N146" t="inlineStr">
@@ -7059,7 +7059,7 @@
       </c>
       <c r="L147" t="inlineStr">
         <is>
-          <t>Gestor de intereses</t>
+          <t>Lobista</t>
         </is>
       </c>
       <c r="M147" t="inlineStr">
@@ -8166,7 +8166,7 @@
       </c>
       <c r="M169" t="inlineStr">
         <is>
-          <t>asociacion de isapres de chile</t>
+          <t>ESENCIAL S.A.</t>
         </is>
       </c>
       <c r="N169" t="inlineStr">
@@ -13537,7 +13537,7 @@
       </c>
       <c r="L284" t="inlineStr">
         <is>
-          <t>Gestor de intereses</t>
+          <t>Lobista</t>
         </is>
       </c>
       <c r="M284" t="inlineStr">
@@ -13936,7 +13936,7 @@
       </c>
       <c r="M292" t="inlineStr">
         <is>
-          <t>asociacion de isapres de chile</t>
+          <t>ESENCIAL S.A.</t>
         </is>
       </c>
       <c r="N292" t="inlineStr">
@@ -14643,7 +14643,7 @@
       </c>
       <c r="L306" t="inlineStr">
         <is>
-          <t>Gestor de intereses</t>
+          <t>Lobista</t>
         </is>
       </c>
       <c r="M306" t="inlineStr">
@@ -15397,7 +15397,7 @@
       </c>
       <c r="M322" t="inlineStr">
         <is>
-          <t>Esencial S.A.</t>
+          <t>ESENCIAL S.A.</t>
         </is>
       </c>
       <c r="N322" t="inlineStr">
@@ -15429,7 +15429,7 @@
       </c>
       <c r="M323" t="inlineStr">
         <is>
-          <t>asociacion de isapres de chile</t>
+          <t>ESENCIAL S.A.</t>
         </is>
       </c>
       <c r="N323" t="inlineStr">
@@ -15664,7 +15664,7 @@
       </c>
       <c r="L327" t="inlineStr">
         <is>
-          <t>Gestor de intereses</t>
+          <t>Lobista</t>
         </is>
       </c>
       <c r="M327" t="inlineStr">
@@ -16458,7 +16458,7 @@
       </c>
       <c r="L343" t="inlineStr">
         <is>
-          <t>Gestor de intereses</t>
+          <t>Lobista</t>
         </is>
       </c>
       <c r="M343" t="inlineStr">
@@ -16858,7 +16858,7 @@
       </c>
       <c r="L351" t="inlineStr">
         <is>
-          <t>Gestor de intereses</t>
+          <t>Lobista</t>
         </is>
       </c>
       <c r="M351" t="inlineStr">
@@ -18426,7 +18426,7 @@
       </c>
       <c r="L385" t="inlineStr">
         <is>
-          <t>Gestor de intereses</t>
+          <t>Lobista</t>
         </is>
       </c>
       <c r="M385" t="inlineStr">
@@ -19662,7 +19662,7 @@
       </c>
       <c r="L411" t="inlineStr">
         <is>
-          <t>Gestor de intereses</t>
+          <t>Lobista</t>
         </is>
       </c>
       <c r="M411" t="inlineStr">
@@ -19769,7 +19769,7 @@
       </c>
       <c r="M413" t="inlineStr">
         <is>
-          <t>asociacion de isapres de chile</t>
+          <t>ESENCIAL S.A.</t>
         </is>
       </c>
       <c r="N413" t="inlineStr">
@@ -19801,7 +19801,7 @@
       </c>
       <c r="M414" t="inlineStr">
         <is>
-          <t>Esencial S.A.</t>
+          <t>ESENCIAL S.A.</t>
         </is>
       </c>
       <c r="N414" t="inlineStr">

</xml_diff>